<commit_message>
Changes to purchase_plan.xlsx --new purchases from mouser, seeedstudio, and ebay
</commit_message>
<xml_diff>
--- a/Purchase plan-Sep_2015.xlsx
+++ b/Purchase plan-Sep_2015.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26405"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16340" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prototype-Mechanical" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,17 @@
     <sheet name="Motion capture" sheetId="11" r:id="rId9"/>
     <sheet name="Help" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="232">
   <si>
     <t>Item</t>
   </si>
@@ -695,13 +700,37 @@
   </si>
   <si>
     <t>Submitted recipt</t>
+  </si>
+  <si>
+    <t>Cart Naming:</t>
+  </si>
+  <si>
+    <t>Use the first and last letter of the supplier name aumented by DDMMYY</t>
+  </si>
+  <si>
+    <t>seeedstudio</t>
+  </si>
+  <si>
+    <t>Amount (USD)</t>
+  </si>
+  <si>
+    <t>SO030116</t>
+  </si>
+  <si>
+    <t>Seeedstudio</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>10 X 10 cm custom PCB with stencil (total price includes shipping cost)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,6 +741,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -776,8 +821,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -807,11 +908,67 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="57">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -870,7 +1027,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -905,7 +1062,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1120,15 +1277,15 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="22.6328125" customWidth="1"/>
-    <col min="4" max="4" width="56.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.08984375" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
+    <col min="4" max="4" width="56.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1154,7 +1311,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
@@ -1178,7 +1335,7 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="15"/>
       <c r="B3" s="14"/>
       <c r="C3" t="s">
@@ -1198,7 +1355,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="15"/>
       <c r="B4" s="14"/>
       <c r="C4" t="s">
@@ -1211,7 +1368,7 @@
         <v>21.24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="15"/>
       <c r="B5" s="14"/>
       <c r="C5" t="s">
@@ -1222,86 +1379,106 @@
         <v>35.58</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:8" s="1" customFormat="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="B1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="5"/>
       <c r="B2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" s="7"/>
       <c r="B3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="13"/>
       <c r="B6" t="s">
         <v>223</v>
       </c>
     </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:DG61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.26953125" customWidth="1"/>
+    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1330,7 +1507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" s="16" t="s">
         <v>187</v>
       </c>
@@ -1360,7 +1537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" s="16"/>
       <c r="B3" s="14"/>
       <c r="C3" s="4" t="s">
@@ -1383,7 +1560,7 @@
         <v>1.95</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9">
       <c r="A4" s="16"/>
       <c r="B4" s="14"/>
       <c r="C4" t="s">
@@ -1406,7 +1583,7 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" s="16"/>
       <c r="B5" s="14"/>
       <c r="C5" t="s">
@@ -1429,7 +1606,7 @@
         <v>29.95</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" s="16"/>
       <c r="B6" s="14"/>
       <c r="C6" t="s">
@@ -1452,7 +1629,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" s="16"/>
       <c r="B7" s="14"/>
       <c r="C7" t="s">
@@ -1475,7 +1652,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="16"/>
       <c r="B8" s="14"/>
       <c r="C8" t="s">
@@ -1498,7 +1675,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" s="16"/>
       <c r="B9" s="14"/>
       <c r="C9" t="s">
@@ -1521,7 +1698,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9">
       <c r="A10" s="16"/>
       <c r="B10" s="14"/>
       <c r="C10" t="s">
@@ -1544,7 +1721,7 @@
         <v>9.9499999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" s="16"/>
       <c r="B11" s="14"/>
       <c r="C11" t="s">
@@ -1567,7 +1744,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="A12" s="16"/>
       <c r="B12" s="14"/>
       <c r="C12" t="s">
@@ -1590,7 +1767,7 @@
         <v>9.9499999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="A13" s="16"/>
       <c r="C13" t="s">
         <v>144</v>
@@ -1612,7 +1789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="A14" s="16"/>
       <c r="C14" t="s">
         <v>170</v>
@@ -1634,8 +1811,8 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" s="1" customFormat="1"/>
+    <row r="16" spans="1:9">
       <c r="A16" s="15" t="s">
         <v>188</v>
       </c>
@@ -1662,7 +1839,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8">
       <c r="A17" s="15"/>
       <c r="B17" s="14"/>
       <c r="C17" t="s">
@@ -1685,7 +1862,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8">
       <c r="A18" s="15"/>
       <c r="B18" s="14"/>
       <c r="C18" t="s">
@@ -1708,10 +1885,10 @@
         <v>2.0099999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="1" customFormat="1">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8">
       <c r="A20" s="17" t="s">
         <v>189</v>
       </c>
@@ -1738,7 +1915,7 @@
         <v>30.599999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8">
       <c r="A21" s="17"/>
       <c r="B21" s="14"/>
       <c r="C21" t="s">
@@ -1761,7 +1938,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8">
       <c r="A22" s="17"/>
       <c r="B22" s="14"/>
       <c r="C22" t="s">
@@ -1784,7 +1961,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" t="s">
@@ -1807,7 +1984,7 @@
         <v>5.6499999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" t="s">
@@ -1830,7 +2007,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" t="s">
@@ -1853,7 +2030,7 @@
         <v>5.92</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" t="s">
@@ -1876,7 +2053,7 @@
         <v>5.5500000000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" t="s">
@@ -1899,7 +2076,7 @@
         <v>7.7200000000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" t="s">
@@ -1922,7 +2099,7 @@
         <v>8.6199999999999992</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" t="s">
@@ -1945,7 +2122,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8">
       <c r="A30" s="17"/>
       <c r="B30" s="14"/>
       <c r="C30" t="s">
@@ -1968,7 +2145,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8">
       <c r="A31" s="17"/>
       <c r="B31" s="14"/>
       <c r="C31" t="s">
@@ -1991,7 +2168,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8">
       <c r="A32" s="17"/>
       <c r="B32" s="14"/>
       <c r="C32" t="s">
@@ -2014,7 +2191,7 @@
         <v>1.9500000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8">
       <c r="A33" s="17"/>
       <c r="B33" s="14"/>
       <c r="C33" t="s">
@@ -2037,7 +2214,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8">
       <c r="A34" s="17"/>
       <c r="B34" s="14"/>
       <c r="C34" t="s">
@@ -2060,7 +2237,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8">
       <c r="A35" s="17"/>
       <c r="B35" s="14"/>
       <c r="C35" t="s">
@@ -2083,7 +2260,7 @@
         <v>3.7800000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8">
       <c r="A36" s="17"/>
       <c r="B36" s="14"/>
       <c r="C36" t="s">
@@ -2106,7 +2283,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8">
       <c r="A37" s="17"/>
       <c r="B37" s="14"/>
       <c r="C37" t="s">
@@ -2129,7 +2306,7 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8">
       <c r="A38" s="17"/>
       <c r="B38" s="14"/>
       <c r="C38" t="s">
@@ -2152,7 +2329,7 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8">
       <c r="A39" s="17"/>
       <c r="B39" s="14"/>
       <c r="C39" t="s">
@@ -2175,7 +2352,7 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8">
       <c r="A40" s="17"/>
       <c r="B40" s="14"/>
       <c r="C40" t="s">
@@ -2198,7 +2375,7 @@
         <v>4.0699999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8">
       <c r="A41" s="17"/>
       <c r="B41" s="14"/>
       <c r="C41" t="s">
@@ -2221,7 +2398,7 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8">
       <c r="A42" s="17"/>
       <c r="B42" s="14"/>
       <c r="C42" t="s">
@@ -2244,7 +2421,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8">
       <c r="A43" s="17"/>
       <c r="B43" s="14"/>
       <c r="C43" t="s">
@@ -2267,7 +2444,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8">
       <c r="A44" s="17"/>
       <c r="B44" s="14"/>
       <c r="C44" t="s">
@@ -2290,7 +2467,7 @@
         <v>13.700000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8">
       <c r="A45" s="17"/>
       <c r="B45" s="14"/>
       <c r="C45" t="s">
@@ -2313,7 +2490,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8">
       <c r="A46" s="17"/>
       <c r="B46" s="14"/>
       <c r="C46" t="s">
@@ -2336,7 +2513,7 @@
         <v>13.600000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8">
       <c r="A47" s="17"/>
       <c r="B47" s="14"/>
       <c r="C47" t="s">
@@ -2359,7 +2536,7 @@
         <v>16.599999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8">
       <c r="A48" s="17"/>
       <c r="B48" s="14"/>
       <c r="C48" t="s">
@@ -2382,7 +2559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:111">
       <c r="A49" s="17"/>
       <c r="B49" s="14"/>
       <c r="C49" t="s">
@@ -2405,7 +2582,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:111">
       <c r="A50" s="17"/>
       <c r="B50" s="14"/>
       <c r="C50" t="s">
@@ -2428,7 +2605,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:111">
       <c r="A51" s="17"/>
       <c r="B51" s="14"/>
       <c r="C51" t="s">
@@ -2451,7 +2628,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:111">
       <c r="A52" s="17"/>
       <c r="B52" s="14"/>
       <c r="C52" t="s">
@@ -2474,7 +2651,7 @@
         <v>16.200000000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:111">
       <c r="A53" s="17"/>
       <c r="B53" s="3"/>
       <c r="C53" t="s">
@@ -2497,11 +2674,11 @@
         <v>5.88</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:111">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:111" s="1" customFormat="1"/>
+    <row r="56" spans="1:111">
       <c r="A56" s="17" t="s">
         <v>190</v>
       </c>
@@ -2525,7 +2702,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:111">
       <c r="A57" s="17"/>
       <c r="B57" s="14"/>
       <c r="C57" t="s">
@@ -2545,7 +2722,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:111">
       <c r="A58" s="17"/>
       <c r="B58" s="14"/>
       <c r="C58" t="s">
@@ -2563,6 +2740,139 @@
       <c r="H58">
         <f>G58*F58</f>
         <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:111">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="1"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+      <c r="Y60" s="1"/>
+      <c r="Z60" s="1"/>
+      <c r="AA60" s="1"/>
+      <c r="AB60" s="1"/>
+      <c r="AC60" s="1"/>
+      <c r="AD60" s="1"/>
+      <c r="AE60" s="1"/>
+      <c r="AF60" s="1"/>
+      <c r="AG60" s="1"/>
+      <c r="AH60" s="1"/>
+      <c r="AI60" s="1"/>
+      <c r="AJ60" s="1"/>
+      <c r="AK60" s="1"/>
+      <c r="AL60" s="1"/>
+      <c r="AM60" s="1"/>
+      <c r="AN60" s="1"/>
+      <c r="AO60" s="1"/>
+      <c r="AP60" s="1"/>
+      <c r="AQ60" s="1"/>
+      <c r="AR60" s="1"/>
+      <c r="AS60" s="1"/>
+      <c r="AT60" s="1"/>
+      <c r="AU60" s="1"/>
+      <c r="AV60" s="1"/>
+      <c r="AW60" s="1"/>
+      <c r="AX60" s="1"/>
+      <c r="AY60" s="1"/>
+      <c r="AZ60" s="1"/>
+      <c r="BA60" s="1"/>
+      <c r="BB60" s="1"/>
+      <c r="BC60" s="1"/>
+      <c r="BD60" s="1"/>
+      <c r="BE60" s="1"/>
+      <c r="BF60" s="1"/>
+      <c r="BG60" s="1"/>
+      <c r="BH60" s="1"/>
+      <c r="BI60" s="1"/>
+      <c r="BJ60" s="1"/>
+      <c r="BK60" s="1"/>
+      <c r="BL60" s="1"/>
+      <c r="BM60" s="1"/>
+      <c r="BN60" s="1"/>
+      <c r="BO60" s="1"/>
+      <c r="BP60" s="1"/>
+      <c r="BQ60" s="1"/>
+      <c r="BR60" s="1"/>
+      <c r="BS60" s="1"/>
+      <c r="BT60" s="1"/>
+      <c r="BU60" s="1"/>
+      <c r="BV60" s="1"/>
+      <c r="BW60" s="1"/>
+      <c r="BX60" s="1"/>
+      <c r="BY60" s="1"/>
+      <c r="BZ60" s="1"/>
+      <c r="CA60" s="1"/>
+      <c r="CB60" s="1"/>
+      <c r="CC60" s="1"/>
+      <c r="CD60" s="1"/>
+      <c r="CE60" s="1"/>
+      <c r="CF60" s="1"/>
+      <c r="CG60" s="1"/>
+      <c r="CH60" s="1"/>
+      <c r="CI60" s="1"/>
+      <c r="CJ60" s="1"/>
+      <c r="CK60" s="1"/>
+      <c r="CL60" s="1"/>
+      <c r="CM60" s="1"/>
+      <c r="CN60" s="1"/>
+      <c r="CO60" s="1"/>
+      <c r="CP60" s="1"/>
+      <c r="CQ60" s="1"/>
+      <c r="CR60" s="1"/>
+      <c r="CS60" s="1"/>
+      <c r="CT60" s="1"/>
+      <c r="CU60" s="1"/>
+      <c r="CV60" s="1"/>
+      <c r="CW60" s="1"/>
+      <c r="CX60" s="1"/>
+      <c r="CY60" s="1"/>
+      <c r="CZ60" s="1"/>
+      <c r="DA60" s="1"/>
+      <c r="DB60" s="1"/>
+      <c r="DC60" s="1"/>
+      <c r="DD60" s="1"/>
+      <c r="DE60" s="1"/>
+      <c r="DF60" s="1"/>
+      <c r="DG60" s="1"/>
+    </row>
+    <row r="61" spans="1:111">
+      <c r="A61" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" t="s">
+        <v>229</v>
+      </c>
+      <c r="C61" t="s">
+        <v>230</v>
+      </c>
+      <c r="D61" t="s">
+        <v>231</v>
+      </c>
+      <c r="F61">
+        <v>10</v>
+      </c>
+      <c r="H61">
+        <v>109.34</v>
       </c>
     </row>
   </sheetData>
@@ -2577,7 +2887,12 @@
     <mergeCell ref="A56:A58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2586,20 +2901,20 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="86.90625" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86.875" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2628,7 +2943,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" s="13" t="s">
         <v>187</v>
       </c>
@@ -2655,7 +2970,7 @@
         <v>69.900000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
         <v>191</v>
       </c>
@@ -2677,7 +2992,7 @@
         <v>459.8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9">
       <c r="A4" s="13" t="s">
         <v>187</v>
       </c>
@@ -2702,8 +3017,8 @@
         <v>2.95</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" s="1" customFormat="1"/>
+    <row r="6" spans="1:9">
       <c r="A6" s="17" t="s">
         <v>189</v>
       </c>
@@ -2730,7 +3045,7 @@
         <v>1.419</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" s="17"/>
       <c r="B7" s="14"/>
       <c r="C7" t="s">
@@ -2750,7 +3065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="17"/>
       <c r="B8" s="14"/>
       <c r="C8" t="s">
@@ -2773,7 +3088,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" s="17"/>
       <c r="B9" s="14"/>
       <c r="C9" t="s">
@@ -2803,7 +3118,12 @@
     <mergeCell ref="A6:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2812,20 +3132,20 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="68.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2851,7 +3171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="17" t="s">
         <v>189</v>
       </c>
@@ -2878,7 +3198,7 @@
         <v>2.133</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="17"/>
       <c r="B3" s="14"/>
       <c r="C3" t="s">
@@ -2901,10 +3221,10 @@
         <v>2.63</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="1" customFormat="1">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="16" t="s">
         <v>187</v>
       </c>
@@ -2931,7 +3251,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8">
       <c r="A6" s="16"/>
       <c r="B6" s="14"/>
       <c r="C6" s="9" t="s">
@@ -2954,7 +3274,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="A7" s="16"/>
       <c r="B7" s="14"/>
       <c r="C7" t="s">
@@ -2977,7 +3297,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8">
       <c r="A8" s="16"/>
       <c r="B8" s="14"/>
       <c r="C8" t="s">
@@ -3008,7 +3328,12 @@
     <mergeCell ref="B5:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3020,18 +3345,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.125" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3057,7 +3382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
         <v>192</v>
       </c>
@@ -3083,7 +3408,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3095,18 +3425,18 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3135,7 +3465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
         <v>193</v>
       </c>
@@ -3161,6 +3491,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3172,9 +3507,9 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3205,26 +3540,32 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>194</v>
       </c>
@@ -3238,13 +3579,16 @@
         <v>202</v>
       </c>
       <c r="E1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" t="s">
         <v>213</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7">
       <c r="A2" s="10">
         <v>42117</v>
       </c>
@@ -3257,11 +3601,11 @@
       <c r="D2" t="s">
         <v>78</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>810</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" s="10">
         <v>42264</v>
       </c>
@@ -3274,11 +3618,11 @@
       <c r="D3" t="s">
         <v>203</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" s="10">
         <v>42277</v>
       </c>
@@ -3291,11 +3635,11 @@
       <c r="D4" t="s">
         <v>203</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="10">
         <v>42279</v>
       </c>
@@ -3308,15 +3652,71 @@
       <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>3008</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="10">
+        <v>42430</v>
+      </c>
+      <c r="B6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E6">
+        <v>109.34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="10">
+        <v>42461</v>
+      </c>
+      <c r="B7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7">
+        <v>347.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="10">
+        <v>42461</v>
+      </c>
+      <c r="B8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8">
+        <v>697.19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3328,47 +3728,47 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>208</v>
       </c>
@@ -3376,7 +3776,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>216</v>
       </c>
@@ -3384,33 +3784,38 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2">
       <c r="B17" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2">
       <c r="B18" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2">
       <c r="B19" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2">
       <c r="B20" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2">
       <c r="B21" t="s">
         <v>220</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>